<commit_message>
Added some calendar components
</commit_message>
<xml_diff>
--- a/backend/schedule.xlsx
+++ b/backend/schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdleg\Downloads\Programs\Mac_Calendar\v1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdleg\Downloads\Programs\Mac_Calendar\v1\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB94B89C-B4B8-47D0-AE7A-F3E6D23D1CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68ABE0E-34EB-42C5-8115-EDEB09C5A56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="345" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -3690,7 +3690,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3707,6 +3707,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4025,8 +4026,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J2603"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1652" workbookViewId="0">
-      <selection activeCell="F2601" sqref="F2601"/>
+    <sheetView tabSelected="1" topLeftCell="A1650" workbookViewId="0">
+      <selection activeCell="G2601" sqref="G2601"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5935,7 +5936,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>11</v>
       </c>
@@ -5967,7 +5968,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>11</v>
       </c>
@@ -5999,7 +6000,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>11</v>
       </c>
@@ -6031,7 +6032,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>11</v>
       </c>
@@ -6063,7 +6064,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="66" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -6095,7 +6096,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>11</v>
       </c>
@@ -6127,7 +6128,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -6159,7 +6160,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -6188,7 +6189,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>11</v>
       </c>
@@ -6220,7 +6221,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>11</v>
       </c>
@@ -6249,7 +6250,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>11</v>
       </c>
@@ -6278,7 +6279,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>11</v>
       </c>
@@ -6307,7 +6308,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>11</v>
       </c>
@@ -6336,7 +6337,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>11</v>
       </c>
@@ -6365,7 +6366,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>11</v>
       </c>
@@ -6397,7 +6398,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>11</v>
       </c>
@@ -6426,7 +6427,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>11</v>
       </c>
@@ -6455,7 +6456,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="79" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>11</v>
       </c>
@@ -6484,7 +6485,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="80" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>11</v>
       </c>
@@ -6513,7 +6514,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>11</v>
       </c>
@@ -6545,7 +6546,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>11</v>
       </c>
@@ -6577,7 +6578,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>11</v>
       </c>
@@ -6609,7 +6610,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>11</v>
       </c>
@@ -6641,7 +6642,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>11</v>
       </c>
@@ -6673,7 +6674,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>11</v>
       </c>
@@ -6705,7 +6706,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>11</v>
       </c>
@@ -6737,7 +6738,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>11</v>
       </c>
@@ -6769,7 +6770,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>11</v>
       </c>
@@ -6801,7 +6802,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>11</v>
       </c>
@@ -6833,7 +6834,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>11</v>
       </c>
@@ -6865,7 +6866,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>11</v>
       </c>
@@ -6897,7 +6898,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>11</v>
       </c>
@@ -6929,7 +6930,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>11</v>
       </c>
@@ -6961,7 +6962,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>11</v>
       </c>
@@ -6993,7 +6994,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>11</v>
       </c>
@@ -7025,7 +7026,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>11</v>
       </c>
@@ -7057,7 +7058,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -7089,7 +7090,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>11</v>
       </c>
@@ -7121,7 +7122,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>11</v>
       </c>
@@ -7153,7 +7154,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>11</v>
       </c>
@@ -7185,7 +7186,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>11</v>
       </c>
@@ -7217,7 +7218,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="103" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>11</v>
       </c>
@@ -7249,7 +7250,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="104" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>11</v>
       </c>
@@ -7281,7 +7282,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="105" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>11</v>
       </c>
@@ -7313,7 +7314,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="106" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>11</v>
       </c>
@@ -7345,7 +7346,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="107" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>11</v>
       </c>
@@ -7377,7 +7378,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="108" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>11</v>
       </c>
@@ -7409,7 +7410,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>11</v>
       </c>
@@ -7441,7 +7442,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="110" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>11</v>
       </c>
@@ -7473,7 +7474,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="111" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>11</v>
       </c>
@@ -7505,7 +7506,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="112" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>11</v>
       </c>
@@ -7537,7 +7538,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="113" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>11</v>
       </c>
@@ -7569,7 +7570,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="114" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>11</v>
       </c>
@@ -7601,7 +7602,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="115" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>11</v>
       </c>
@@ -7633,7 +7634,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="116" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>11</v>
       </c>
@@ -7665,7 +7666,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="117" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>11</v>
       </c>
@@ -7697,7 +7698,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="118" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>11</v>
       </c>
@@ -7729,7 +7730,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="119" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>11</v>
       </c>
@@ -7761,7 +7762,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>11</v>
       </c>
@@ -7793,7 +7794,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="121" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>11</v>
       </c>
@@ -7825,7 +7826,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="122" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>11</v>
       </c>
@@ -7857,7 +7858,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="123" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>11</v>
       </c>
@@ -9791,7 +9792,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="184" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>11</v>
       </c>
@@ -9823,7 +9824,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="185" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>11</v>
       </c>
@@ -9855,7 +9856,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="186" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>11</v>
       </c>
@@ -9887,7 +9888,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="187" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>11</v>
       </c>
@@ -9919,7 +9920,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="188" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>11</v>
       </c>
@@ -9951,7 +9952,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="189" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>11</v>
       </c>
@@ -9983,7 +9984,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="190" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>11</v>
       </c>
@@ -10015,7 +10016,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="191" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>11</v>
       </c>
@@ -10047,7 +10048,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="192" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>11</v>
       </c>
@@ -10079,7 +10080,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="193" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>11</v>
       </c>
@@ -10111,7 +10112,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="194" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>11</v>
       </c>
@@ -10143,7 +10144,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="195" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>11</v>
       </c>
@@ -10175,7 +10176,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="196" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>11</v>
       </c>
@@ -10207,7 +10208,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="197" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>11</v>
       </c>
@@ -10239,7 +10240,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="198" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>11</v>
       </c>
@@ -10271,7 +10272,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="199" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>11</v>
       </c>
@@ -10303,7 +10304,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="200" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>11</v>
       </c>
@@ -10335,7 +10336,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="201" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>11</v>
       </c>
@@ -10367,7 +10368,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="202" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>11</v>
       </c>
@@ -10399,7 +10400,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="203" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>11</v>
       </c>
@@ -10431,7 +10432,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="204" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>11</v>
       </c>
@@ -10463,7 +10464,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="205" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>11</v>
       </c>
@@ -10495,7 +10496,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="206" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>11</v>
       </c>
@@ -10527,7 +10528,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="207" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>11</v>
       </c>
@@ -10559,7 +10560,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="208" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>11</v>
       </c>
@@ -10591,7 +10592,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="209" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>11</v>
       </c>
@@ -10623,7 +10624,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="210" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>11</v>
       </c>
@@ -10655,7 +10656,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="211" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>11</v>
       </c>
@@ -10687,7 +10688,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="212" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>11</v>
       </c>
@@ -10719,7 +10720,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="213" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>11</v>
       </c>
@@ -10751,7 +10752,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="214" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>11</v>
       </c>
@@ -10783,7 +10784,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="215" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>11</v>
       </c>
@@ -10815,7 +10816,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="216" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>11</v>
       </c>
@@ -10847,7 +10848,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="217" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>11</v>
       </c>
@@ -10879,7 +10880,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="218" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>11</v>
       </c>
@@ -10911,7 +10912,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="219" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>11</v>
       </c>
@@ -10943,7 +10944,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="220" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>11</v>
       </c>
@@ -10975,7 +10976,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="221" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>11</v>
       </c>
@@ -11007,7 +11008,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="222" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>11</v>
       </c>
@@ -11039,7 +11040,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="223" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>11</v>
       </c>
@@ -11071,7 +11072,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="224" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>11</v>
       </c>
@@ -11103,7 +11104,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="225" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>11</v>
       </c>
@@ -11135,7 +11136,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="226" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>11</v>
       </c>
@@ -11167,7 +11168,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="227" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>11</v>
       </c>
@@ -11199,7 +11200,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="228" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>11</v>
       </c>
@@ -11231,7 +11232,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="229" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>11</v>
       </c>
@@ -11263,7 +11264,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="230" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>11</v>
       </c>
@@ -11295,7 +11296,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="231" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>11</v>
       </c>
@@ -11327,7 +11328,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="232" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>11</v>
       </c>
@@ -11347,7 +11348,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="233" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>11</v>
       </c>
@@ -11379,7 +11380,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="234" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>11</v>
       </c>
@@ -11411,7 +11412,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="235" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>11</v>
       </c>
@@ -11443,7 +11444,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="236" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>11</v>
       </c>
@@ -11475,7 +11476,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="237" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>11</v>
       </c>
@@ -11507,7 +11508,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="238" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>11</v>
       </c>
@@ -11539,7 +11540,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="239" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>11</v>
       </c>
@@ -11571,7 +11572,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="240" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>11</v>
       </c>
@@ -11603,7 +11604,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="241" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>11</v>
       </c>
@@ -11635,7 +11636,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="242" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>11</v>
       </c>
@@ -11667,7 +11668,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="243" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>11</v>
       </c>
@@ -11699,7 +11700,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="244" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>11</v>
       </c>
@@ -11731,7 +11732,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="245" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>11</v>
       </c>
@@ -11763,7 +11764,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="246" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>11</v>
       </c>
@@ -11795,7 +11796,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="247" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>11</v>
       </c>
@@ -11827,7 +11828,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="248" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>11</v>
       </c>
@@ -11859,7 +11860,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="249" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>11</v>
       </c>
@@ -11891,7 +11892,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="250" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>11</v>
       </c>
@@ -11923,7 +11924,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="251" spans="1:10" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:10" ht="15.75" hidden="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>11</v>
       </c>
@@ -52447,7 +52448,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="1538" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1538" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A1538" t="s">
         <v>11</v>
       </c>
@@ -84711,7 +84712,7 @@
       <c r="F2601" t="s">
         <v>36</v>
       </c>
-      <c r="G2601" s="15">
+      <c r="G2601" s="16">
         <v>8.3000000000000007</v>
       </c>
       <c r="H2601" s="15">

</xml_diff>

<commit_message>
Aded math to year 2
</commit_message>
<xml_diff>
--- a/backend/schedule.xlsx
+++ b/backend/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdleg\Downloads\Programs\Mac_Calendar\v1\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0524A217-3626-4124-BDA4-BC23BB3C3872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9D0D90-A494-4A08-BB96-84E8475A3CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2370" yWindow="3630" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -3527,19 +3527,19 @@
     <t>TIME</t>
   </si>
   <si>
-    <t>3R03</t>
-  </si>
-  <si>
     <t>3ES3</t>
   </si>
   <si>
-    <t>Math</t>
-  </si>
-  <si>
     <t>Econ</t>
   </si>
   <si>
     <t>ENG</t>
+  </si>
+  <si>
+    <t>2R03</t>
+  </si>
+  <si>
+    <t>MATH</t>
   </si>
 </sst>
 </file>
@@ -4029,7 +4029,7 @@
   <dimension ref="A1:J2603"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1650" workbookViewId="0">
-      <selection activeCell="B2603" sqref="B2603"/>
+      <selection activeCell="B2601" sqref="B2601"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -84703,10 +84703,10 @@
         <v>1166</v>
       </c>
       <c r="C2601" t="s">
-        <v>1162</v>
+        <v>1165</v>
       </c>
       <c r="D2601" t="s">
-        <v>1164</v>
+        <v>1166</v>
       </c>
       <c r="E2601" t="s">
         <v>15</v>
@@ -84726,13 +84726,13 @@
         <v>2241</v>
       </c>
       <c r="B2603" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="C2603" t="s">
+        <v>1162</v>
+      </c>
+      <c r="D2603" t="s">
         <v>1163</v>
-      </c>
-      <c r="D2603" t="s">
-        <v>1165</v>
       </c>
       <c r="E2603" t="s">
         <v>15</v>

</xml_diff>